<commit_message>
fix coordinates in myt_metdata.xlsx
</commit_message>
<xml_diff>
--- a/myt_metadata.xlsx
+++ b/myt_metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanessa\Documents\Mytilus Project\Code\Mytilus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/github/Mytilus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562D816A-9BBF-4CA6-B3C1-7853DCF7CB08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C18639-42B0-BE46-A45B-C4C03B2C44A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1944" yWindow="1176" windowWidth="10620" windowHeight="8280" xr2:uid="{5920EFEB-4D8A-42A3-A32C-24AF679F328E}"/>
+    <workbookView xWindow="-180" yWindow="1120" windowWidth="22620" windowHeight="16440" xr2:uid="{5920EFEB-4D8A-42A3-A32C-24AF679F328E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>locality</t>
   </si>
@@ -88,25 +88,67 @@
   </si>
   <si>
     <t>China Beach</t>
+  </si>
+  <si>
+    <t>35.604713</t>
+  </si>
+  <si>
+    <t>-121.143064</t>
+  </si>
+  <si>
+    <t>35.289806</t>
+  </si>
+  <si>
+    <t>-120.883968</t>
+  </si>
+  <si>
+    <t>34.460525</t>
+  </si>
+  <si>
+    <t>-120.074125</t>
+  </si>
+  <si>
+    <t>38.731386</t>
+  </si>
+  <si>
+    <t>-123.489816</t>
+  </si>
+  <si>
+    <t>38.304079</t>
+  </si>
+  <si>
+    <t>-123.053742</t>
+  </si>
+  <si>
+    <t>33.716127</t>
+  </si>
+  <si>
+    <t>-118.319394</t>
+  </si>
+  <si>
+    <t>32.847464</t>
+  </si>
+  <si>
+    <t>-117.277691</t>
+  </si>
+  <si>
+    <t>34.387257</t>
+  </si>
+  <si>
+    <t>-119.513572</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF4D5156"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +171,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,18 +489,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73551733-E5C4-4764-8DD7-97B22585C805}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="349" zoomScaleNormal="349" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -481,7 +522,7 @@
         <v>-125.7538</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -492,7 +533,7 @@
         <v>-125.4342</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -503,7 +544,7 @@
         <v>-124.0789</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -514,7 +555,7 @@
         <v>-125.14279999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -525,7 +566,7 @@
         <v>-124.42230000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -536,103 +577,103 @@
         <v>-136.3433</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>34.462763000000002</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-120.06915100000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>35.29</v>
-      </c>
-      <c r="C9">
-        <v>-120.88379999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>33.818899999999999</v>
-      </c>
-      <c r="C10">
-        <v>-118.1987</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>25.985900000000001</v>
-      </c>
-      <c r="C11">
-        <v>-80.122799999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>38.311</v>
-      </c>
-      <c r="C12">
-        <v>-123.06610000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>37.013500000000001</v>
+        <v>37.010500999999998</v>
       </c>
       <c r="C13">
-        <v>-122.19670000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-122.199563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>33.714700000000001</v>
-      </c>
-      <c r="C14">
-        <v>-118.3142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>32.832799999999999</v>
-      </c>
-      <c r="C15">
-        <v>-117.2713</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>34.398899999999998</v>
-      </c>
-      <c r="C16">
-        <v>-119.5185</v>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>